<commit_message>
fix pubmed genbank combined file, the number of records and number of genes should be fetched from features and genes tables.
</commit_message>
<xml_diff>
--- a/OutputData/CCHF/CCHF_Combined_12_12.xlsx
+++ b/OutputData/CCHF/CCHF_Combined_12_12.xlsx
@@ -595,7 +595,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>NP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>NA (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (17)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -862,7 +862,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>NA (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>ENVELOPE (1), RDRP (1), NP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>L (6), NUCLEOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>L (4), NUCLEOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1582,7 +1582,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>L (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (8), NUCLEOPROTEIN (7)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1853,7 +1853,7 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>N-PROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -2035,7 +2035,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEINS (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2211,7 +2211,7 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2300,7 +2300,7 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>ENVELOPE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2389,7 +2389,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2478,7 +2478,7 @@
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (11)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2565,7 +2565,7 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2652,7 +2652,7 @@
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2834,7 +2834,7 @@
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>ENVELOPE (2), NUCLEOCAPSID (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>NA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3190,7 +3190,7 @@
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>GPC (2), NP (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3279,7 +3279,7 @@
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>NA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -3368,7 +3368,7 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>L (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3461,7 +3461,7 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>L (4), NUCLEOCAPSID (3), ENVELOPE (2), GPC (2), NP (2), POLYPROTEIN (1), NA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3550,7 +3550,7 @@
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3639,7 +3639,7 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>ENVELOPE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3817,7 +3817,7 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>NA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3906,7 +3906,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3995,7 +3995,7 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>POLYPROTEIN (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>CAPSID (28), NA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -4177,7 +4177,7 @@
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>RDRP (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -4266,7 +4266,7 @@
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>RDRP (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -4359,7 +4359,7 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>RDRP (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -4448,7 +4448,7 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>NA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4541,7 +4541,7 @@
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (23)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -4634,7 +4634,7 @@
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>ENVELOPE (11)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4723,7 +4723,7 @@
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4812,7 +4812,7 @@
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2), RNA-DEPENDENT (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4901,7 +4901,7 @@
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (8)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>ENVELOPE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -5083,7 +5083,7 @@
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -5172,7 +5172,7 @@
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -5350,7 +5350,7 @@
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -5439,7 +5439,7 @@
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>NA (12)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>ENVELOPE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -5617,7 +5617,7 @@
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -5706,7 +5706,7 @@
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>NA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -5795,7 +5795,7 @@
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>RDRP (1), GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -5884,7 +5884,7 @@
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5973,7 +5973,7 @@
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>N (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -6066,7 +6066,7 @@
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>ENVELOPE (14)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -6155,7 +6155,7 @@
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -6244,7 +6244,7 @@
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (4), POLYMERASE (1), GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -6333,7 +6333,7 @@
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -6426,7 +6426,7 @@
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>ENVELOPE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -6515,7 +6515,7 @@
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -6604,7 +6604,7 @@
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>N (1), G (1), L (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -6786,7 +6786,7 @@
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -6875,7 +6875,7 @@
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>GP (14), L (14), N (14)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -6964,7 +6964,7 @@
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -7053,7 +7053,7 @@
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -7142,7 +7142,7 @@
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -7231,7 +7231,7 @@
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (9), NUCLEOPROTEIN, NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -7320,7 +7320,7 @@
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -7409,7 +7409,7 @@
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>S (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -7498,7 +7498,7 @@
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -7591,7 +7591,7 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -7680,7 +7680,7 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -7769,7 +7769,7 @@
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -7862,7 +7862,7 @@
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -7955,7 +7955,7 @@
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>N (5), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -8044,7 +8044,7 @@
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -8133,7 +8133,7 @@
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -8226,7 +8226,7 @@
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -8315,7 +8315,7 @@
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>S (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
@@ -8404,7 +8404,7 @@
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>S (6)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
@@ -8493,7 +8493,7 @@
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (4), NUCLEOCAPSID (4), GLYCOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
@@ -8582,7 +8582,7 @@
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>RNA (3), ENVELOPE (3), NUCLEOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
@@ -8671,7 +8671,7 @@
       </c>
       <c r="O92" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P92" t="inlineStr">
@@ -8760,7 +8760,7 @@
       </c>
       <c r="O93" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (446), ENVELOPE (437), RNA-DEPENDENT (416)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P93" t="inlineStr">
@@ -8849,7 +8849,7 @@
       </c>
       <c r="O94" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (7), ENVELOPE (7), NUCLEOCAPSID (7)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P94" t="inlineStr">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="O95" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (232), RNA-DEPENDENT (231), ENVELOPE (231)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P95" t="inlineStr">
@@ -9027,7 +9027,7 @@
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1), GLYCOPROTEIN (1), PUTATIVE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P96" t="inlineStr">
@@ -9120,7 +9120,7 @@
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P97" t="inlineStr">
@@ -9209,7 +9209,7 @@
       </c>
       <c r="O98" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1), RNA-DEPENDENT (1), GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P98" t="inlineStr">
@@ -9298,7 +9298,7 @@
       </c>
       <c r="O99" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P99" t="inlineStr">
@@ -9385,7 +9385,7 @@
       </c>
       <c r="O100" t="inlineStr">
         <is>
-          <t>L (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P100" t="inlineStr">
@@ -9474,7 +9474,7 @@
       </c>
       <c r="O101" t="inlineStr">
         <is>
-          <t>ENVELOPE (1), RNA-DEPENDENT (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P101" t="inlineStr">
@@ -9567,7 +9567,7 @@
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>NA (18)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P102" t="inlineStr">
@@ -9660,7 +9660,7 @@
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1), ENVELOPE (1), RNA-DEPENDENT (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P103" t="inlineStr">
@@ -9753,7 +9753,7 @@
       </c>
       <c r="O104" t="inlineStr">
         <is>
-          <t>ENVELOPE (10)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P104" t="inlineStr">
@@ -9842,7 +9842,7 @@
       </c>
       <c r="O105" t="inlineStr">
         <is>
-          <t>ENVELOPE (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P105" t="inlineStr">
@@ -9937,7 +9937,7 @@
       </c>
       <c r="O106" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (3), RNA-DEPENDENT (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P106" t="inlineStr">
@@ -10028,7 +10028,7 @@
       </c>
       <c r="O107" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (6), ENVELOPE (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P107" t="inlineStr">
@@ -10119,7 +10119,7 @@
       </c>
       <c r="O108" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P108" t="inlineStr">
@@ -10214,7 +10214,7 @@
       </c>
       <c r="O109" t="inlineStr">
         <is>
-          <t>ENVELOPE (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P109" t="inlineStr">
@@ -10305,7 +10305,7 @@
       </c>
       <c r="O110" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P110" t="inlineStr">
@@ -10396,7 +10396,7 @@
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>STRUCTURAL (9)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P111" t="inlineStr">
@@ -10491,7 +10491,7 @@
       </c>
       <c r="O112" t="inlineStr">
         <is>
-          <t>S (6)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P112" t="inlineStr">
@@ -10586,7 +10586,7 @@
       </c>
       <c r="O113" t="inlineStr">
         <is>
-          <t>GPC (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P113" t="inlineStr">
@@ -10681,7 +10681,7 @@
       </c>
       <c r="O114" t="inlineStr">
         <is>
-          <t>NA (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P114" t="inlineStr">
@@ -10776,7 +10776,7 @@
       </c>
       <c r="O115" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (4), RNA-DEPENDENT (4), NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P115" t="inlineStr">
@@ -10871,7 +10871,7 @@
       </c>
       <c r="O116" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P116" t="inlineStr">
@@ -10962,7 +10962,7 @@
       </c>
       <c r="O117" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1), NA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P117" t="inlineStr">
@@ -11049,7 +11049,7 @@
       </c>
       <c r="O118" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (5), GLYCOPROTEIN (5), RNA-DIRECTED (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P118" t="inlineStr">
@@ -11140,7 +11140,7 @@
       </c>
       <c r="O119" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (12)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P119" t="inlineStr">
@@ -11235,7 +11235,7 @@
       </c>
       <c r="O120" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P120" t="inlineStr">
@@ -11330,7 +11330,7 @@
       </c>
       <c r="O121" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P121" t="inlineStr">
@@ -11425,7 +11425,7 @@
       </c>
       <c r="O122" t="inlineStr">
         <is>
-          <t>N (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P122" t="inlineStr">
@@ -11516,7 +11516,7 @@
       </c>
       <c r="O123" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (18), RNA-DEPENDENT (14), ENVELOPE (12)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P123" t="inlineStr">
@@ -11607,7 +11607,7 @@
       </c>
       <c r="O124" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P124" t="inlineStr">
@@ -11698,7 +11698,7 @@
       </c>
       <c r="O125" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), ENVELOPE (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P125" t="inlineStr">
@@ -11789,7 +11789,7 @@
       </c>
       <c r="O126" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P126" t="inlineStr">
@@ -11884,7 +11884,7 @@
       </c>
       <c r="O127" t="inlineStr">
         <is>
-          <t>N-PROTEIN (9), N (3), NA (2), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P127" t="inlineStr">
@@ -11975,7 +11975,7 @@
       </c>
       <c r="O128" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2), ENVELOPE (2), RNA-DEPENDENT (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P128" t="inlineStr">
@@ -12066,7 +12066,7 @@
       </c>
       <c r="O129" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P129" t="inlineStr">
@@ -12157,7 +12157,7 @@
       </c>
       <c r="O130" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1), ENVELOPE (1), TRANSCRIPTASE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P130" t="inlineStr">
@@ -12252,7 +12252,7 @@
       </c>
       <c r="O131" t="inlineStr">
         <is>
-          <t>NA (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P131" t="inlineStr">
@@ -12347,7 +12347,7 @@
       </c>
       <c r="O132" t="inlineStr">
         <is>
-          <t>N (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P132" t="inlineStr">
@@ -12438,7 +12438,7 @@
       </c>
       <c r="O133" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (6)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P133" t="inlineStr">
@@ -12529,7 +12529,7 @@
       </c>
       <c r="O134" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (23), L (23), NUCLEOCAPSID (14)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P134" t="inlineStr">
@@ -12624,7 +12624,7 @@
       </c>
       <c r="O135" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (39)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P135" t="inlineStr">
@@ -12715,7 +12715,7 @@
       </c>
       <c r="O136" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P136" t="inlineStr">
@@ -12810,7 +12810,7 @@
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (36), NA (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P137" t="inlineStr">
@@ -12905,7 +12905,7 @@
       </c>
       <c r="O138" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P138" t="inlineStr">
@@ -13000,7 +13000,7 @@
       </c>
       <c r="O139" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (5), GLYCOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P139" t="inlineStr">
@@ -13095,7 +13095,7 @@
       </c>
       <c r="O140" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (5), GLYCOPROTEIN (5), NUCLEOPROTEIN (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P140" t="inlineStr">
@@ -13186,7 +13186,7 @@
       </c>
       <c r="O141" t="inlineStr">
         <is>
-          <t>S (52)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P141" t="inlineStr">
@@ -13277,7 +13277,7 @@
       </c>
       <c r="O142" t="inlineStr">
         <is>
-          <t>NP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P142" t="inlineStr">
@@ -13368,7 +13368,7 @@
       </c>
       <c r="O143" t="inlineStr">
         <is>
-          <t>NP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P143" t="inlineStr">
@@ -13459,7 +13459,7 @@
       </c>
       <c r="O144" t="inlineStr">
         <is>
-          <t>MEMBRANE (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P144" t="inlineStr">
@@ -13546,7 +13546,7 @@
       </c>
       <c r="O145" t="inlineStr">
         <is>
-          <t>ENVELOPE (1), RNA-DEPENDENT (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P145" t="inlineStr">
@@ -13633,7 +13633,7 @@
       </c>
       <c r="O146" t="inlineStr">
         <is>
-          <t>ENVELOPE (1), RDRP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P146" t="inlineStr">
@@ -13724,7 +13724,7 @@
       </c>
       <c r="O147" t="inlineStr">
         <is>
-          <t>L (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P147" t="inlineStr">
@@ -13815,7 +13815,7 @@
       </c>
       <c r="O148" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P148" t="inlineStr">
@@ -13906,7 +13906,7 @@
       </c>
       <c r="O149" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (44), CAPSID (28), GLYCOPROTEIN (6), NA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P149" t="inlineStr">
@@ -14001,7 +14001,7 @@
       </c>
       <c r="O150" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P150" t="inlineStr">
@@ -14092,7 +14092,7 @@
       </c>
       <c r="O151" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (6)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P151" t="inlineStr">
@@ -14179,7 +14179,7 @@
       </c>
       <c r="O152" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P152" t="inlineStr">
@@ -14274,7 +14274,7 @@
       </c>
       <c r="O153" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (6)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P153" t="inlineStr">
@@ -14365,7 +14365,7 @@
       </c>
       <c r="O154" t="inlineStr">
         <is>
-          <t>N (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P154" t="inlineStr">
@@ -14460,7 +14460,7 @@
       </c>
       <c r="O155" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P155" t="inlineStr">
@@ -14551,7 +14551,7 @@
       </c>
       <c r="O156" t="inlineStr">
         <is>
-          <t>RNA (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P156" t="inlineStr">
@@ -14642,7 +14642,7 @@
       </c>
       <c r="O157" t="inlineStr">
         <is>
-          <t>N (15)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P157" t="inlineStr">
@@ -14737,7 +14737,7 @@
       </c>
       <c r="O158" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P158" t="inlineStr">
@@ -14828,7 +14828,7 @@
       </c>
       <c r="O159" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (23), GLYCOPROTEIN (23), RNA-DEPENDENT (23)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P159" t="inlineStr">
@@ -14919,7 +14919,7 @@
       </c>
       <c r="O160" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (41), GLYCOPROTEINS (41), RNA-DEPENDENT (41)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P160" t="inlineStr">
@@ -15014,7 +15014,7 @@
       </c>
       <c r="O161" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2), ENVELOPE (2), RNA-DEPENDENT (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P161" t="inlineStr">
@@ -15105,7 +15105,7 @@
       </c>
       <c r="O162" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (9), NUCLEOCAPSID (6), ENVELOPE (1), NUCLEOPROTEIN (1), GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P162" t="inlineStr">
@@ -15200,7 +15200,7 @@
       </c>
       <c r="O163" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (12), GLYCOPROTEIN (12), RNA-DEPENDENT (12)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P163" t="inlineStr">
@@ -15295,7 +15295,7 @@
       </c>
       <c r="O164" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (6), VIRAL (1), GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P164" t="inlineStr">
@@ -15390,7 +15390,7 @@
       </c>
       <c r="O165" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P165" t="inlineStr">
@@ -15485,7 +15485,7 @@
       </c>
       <c r="O166" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P166" t="inlineStr">
@@ -15580,7 +15580,7 @@
       </c>
       <c r="O167" t="inlineStr">
         <is>
-          <t>RNA (1), ENVELOPE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P167" t="inlineStr">
@@ -15675,7 +15675,7 @@
       </c>
       <c r="O168" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P168" t="inlineStr">
@@ -15762,7 +15762,7 @@
       </c>
       <c r="O169" t="inlineStr">
         <is>
-          <t>ENVELOPE (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P169" t="inlineStr">
@@ -15857,7 +15857,7 @@
       </c>
       <c r="O170" t="inlineStr">
         <is>
-          <t>S (35), NP (13), GLYCOPROTEIN (12), ENVELOPE (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P170" t="inlineStr">
@@ -15944,7 +15944,7 @@
       </c>
       <c r="O171" t="inlineStr">
         <is>
-          <t>NP (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P171" t="inlineStr">
@@ -16039,7 +16039,7 @@
       </c>
       <c r="O172" t="inlineStr">
         <is>
-          <t>S (35), GLYCOPROTEIN (12), NP (11), ENVELOPE (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P172" t="inlineStr">
@@ -16134,7 +16134,7 @@
       </c>
       <c r="O173" t="inlineStr">
         <is>
-          <t>S (35), NP (13), GLYCOPROTEIN (12), ENVELOPE (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P173" t="inlineStr">
@@ -16221,7 +16221,7 @@
       </c>
       <c r="O174" t="inlineStr">
         <is>
-          <t>ENVELOPE (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P174" t="inlineStr">
@@ -16308,7 +16308,7 @@
       </c>
       <c r="O175" t="inlineStr">
         <is>
-          <t>ENVELOPE (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P175" t="inlineStr">
@@ -16399,7 +16399,7 @@
       </c>
       <c r="O176" t="inlineStr">
         <is>
-          <t>ENVELOPE (6)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P176" t="inlineStr">
@@ -16494,7 +16494,7 @@
       </c>
       <c r="O177" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P177" t="inlineStr">
@@ -16589,7 +16589,7 @@
       </c>
       <c r="O178" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (12), RNA (12), ENVELOPE (12)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P178" t="inlineStr">
@@ -16684,7 +16684,7 @@
       </c>
       <c r="O179" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (7), GLYCOPROTEIN (3), NUCLEOCAPSID (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P179" t="inlineStr">
@@ -16779,7 +16779,7 @@
       </c>
       <c r="O180" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1), GLYCOPROTEIN (1), RNA-DEPENDENT (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P180" t="inlineStr">
@@ -16874,7 +16874,7 @@
       </c>
       <c r="O181" t="inlineStr">
         <is>
-          <t>S (11)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P181" t="inlineStr">
@@ -16969,7 +16969,7 @@
       </c>
       <c r="O182" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (82), GLYCOPROTEIN (52)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P182" t="inlineStr">
@@ -17064,7 +17064,7 @@
       </c>
       <c r="O183" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P183" t="inlineStr">
@@ -17159,7 +17159,7 @@
       </c>
       <c r="O184" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2), GLYCOPROTEIN (2), RNA-DEPENDENT (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P184" t="inlineStr">
@@ -17250,7 +17250,7 @@
       </c>
       <c r="O185" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (10)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P185" t="inlineStr">
@@ -17345,7 +17345,7 @@
       </c>
       <c r="O186" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P186" t="inlineStr">
@@ -17436,7 +17436,7 @@
       </c>
       <c r="O187" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P187" t="inlineStr">
@@ -17523,7 +17523,7 @@
       </c>
       <c r="O188" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (25), NA (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P188" t="inlineStr">
@@ -17618,7 +17618,7 @@
       </c>
       <c r="O189" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P189" t="inlineStr">
@@ -17713,7 +17713,7 @@
       </c>
       <c r="O190" t="inlineStr">
         <is>
-          <t>STRUCTURAL (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P190" t="inlineStr">
@@ -17808,7 +17808,7 @@
       </c>
       <c r="O191" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (1), NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P191" t="inlineStr">
@@ -17903,7 +17903,7 @@
       </c>
       <c r="O192" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (10), GLYCOPROTEIN (10), L (10)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P192" t="inlineStr">
@@ -17994,7 +17994,7 @@
       </c>
       <c r="O193" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P193" t="inlineStr">
@@ -18089,7 +18089,7 @@
       </c>
       <c r="O194" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (2), GLYCOPROTEIN (2), NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P194" t="inlineStr">
@@ -18180,7 +18180,7 @@
       </c>
       <c r="O195" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1), GLYCOPROTEIN (1), RNA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P195" t="inlineStr">
@@ -18275,7 +18275,7 @@
       </c>
       <c r="O196" t="inlineStr">
         <is>
-          <t>PUTATIVE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P196" t="inlineStr">
@@ -18366,7 +18366,7 @@
       </c>
       <c r="O197" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P197" t="inlineStr">
@@ -18461,7 +18461,7 @@
       </c>
       <c r="O198" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (3), GLYCOPROTEIN (3), NUCLEOCAPSID (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P198" t="inlineStr">
@@ -18552,7 +18552,7 @@
       </c>
       <c r="O199" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (3), GLYCOPROTEIN (3), RNA-DEPENDENT (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P199" t="inlineStr">
@@ -18643,7 +18643,7 @@
       </c>
       <c r="O200" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (11)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P200" t="inlineStr">
@@ -18738,7 +18738,7 @@
       </c>
       <c r="O201" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (11), GLYCOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P201" t="inlineStr">
@@ -18829,7 +18829,7 @@
       </c>
       <c r="O202" t="inlineStr">
         <is>
-          <t>GPC (19), RNA-DEPENDENT (8), NUCLEOCAPSID (8)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P202" t="inlineStr">
@@ -18916,7 +18916,7 @@
       </c>
       <c r="O203" t="inlineStr">
         <is>
-          <t>S (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P203" t="inlineStr">
@@ -19007,7 +19007,7 @@
       </c>
       <c r="O204" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (10), GPC (9), RNA-DEPENDENT (9), NUCLEOCAPSID (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P204" t="inlineStr">
@@ -19098,7 +19098,7 @@
       </c>
       <c r="O205" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (3), NUCLEOCAPSID (2), L (2), STRUCTURAL (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P205" t="inlineStr">
@@ -19193,7 +19193,7 @@
       </c>
       <c r="O206" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P206" t="inlineStr">
@@ -19284,7 +19284,7 @@
       </c>
       <c r="O207" t="inlineStr">
         <is>
-          <t>N (1), GLYCOPROTEIN (1), RDRP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P207" t="inlineStr">
@@ -19375,7 +19375,7 @@
       </c>
       <c r="O208" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P208" t="inlineStr">
@@ -19470,7 +19470,7 @@
       </c>
       <c r="O209" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1), NA (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P209" t="inlineStr">
@@ -19561,7 +19561,7 @@
       </c>
       <c r="O210" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (4), ENVELOPE (4), RDRP (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P210" t="inlineStr">
@@ -19652,7 +19652,7 @@
       </c>
       <c r="O211" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (8), GLYCOPROTEIN (8), NUCLEOCAPSID (8)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P211" t="inlineStr">
@@ -19747,7 +19747,7 @@
       </c>
       <c r="O212" t="inlineStr">
         <is>
-          <t>ENVELOPE (25), N (17), NUCLEOCAPSID (16)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P212" t="inlineStr">
@@ -19842,7 +19842,7 @@
       </c>
       <c r="O213" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P213" t="inlineStr">
@@ -19933,7 +19933,7 @@
       </c>
       <c r="O214" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (3), ENVELOPE (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P214" t="inlineStr">
@@ -20024,7 +20024,7 @@
       </c>
       <c r="O215" t="inlineStr">
         <is>
-          <t>RDRP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P215" t="inlineStr">
@@ -20119,7 +20119,7 @@
       </c>
       <c r="O216" t="inlineStr">
         <is>
-          <t>N (17), NUCLEOCAPSID (17), NUCLEOPROTEIN (8), ENVELOPE (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P216" t="inlineStr">
@@ -20214,7 +20214,7 @@
       </c>
       <c r="O217" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (15), ENVELOPE (15), RNA-DEPENDENT (15)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P217" t="inlineStr">
@@ -20305,7 +20305,7 @@
       </c>
       <c r="O218" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P218" t="inlineStr">
@@ -20400,7 +20400,7 @@
       </c>
       <c r="O219" t="inlineStr">
         <is>
-          <t>ENVELOPE (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P219" t="inlineStr">
@@ -20491,7 +20491,7 @@
       </c>
       <c r="O220" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P220" t="inlineStr">
@@ -20582,7 +20582,7 @@
       </c>
       <c r="O221" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P221" t="inlineStr">
@@ -20677,7 +20677,7 @@
       </c>
       <c r="O222" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P222" t="inlineStr">
@@ -20768,7 +20768,7 @@
       </c>
       <c r="O223" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P223" t="inlineStr">
@@ -20859,7 +20859,7 @@
       </c>
       <c r="O224" t="inlineStr">
         <is>
-          <t>GP, GP, GP, GP (1), NP, NP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P224" t="inlineStr">
@@ -20954,7 +20954,7 @@
       </c>
       <c r="O225" t="inlineStr">
         <is>
-          <t>N (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P225" t="inlineStr">
@@ -21045,7 +21045,7 @@
       </c>
       <c r="O226" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (10)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P226" t="inlineStr">
@@ -21136,7 +21136,7 @@
       </c>
       <c r="O227" t="inlineStr">
         <is>
-          <t>L (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P227" t="inlineStr">
@@ -21227,7 +21227,7 @@
       </c>
       <c r="O228" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P228" t="inlineStr">
@@ -21322,7 +21322,7 @@
       </c>
       <c r="O229" t="inlineStr">
         <is>
-          <t>ENVELOPE (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P229" t="inlineStr">
@@ -21417,7 +21417,7 @@
       </c>
       <c r="O230" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (14)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P230" t="inlineStr">
@@ -21512,7 +21512,7 @@
       </c>
       <c r="O231" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P231" t="inlineStr">
@@ -21603,7 +21603,7 @@
       </c>
       <c r="O232" t="inlineStr">
         <is>
-          <t>STRUCTURAL (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P232" t="inlineStr">
@@ -21698,7 +21698,7 @@
       </c>
       <c r="O233" t="inlineStr">
         <is>
-          <t>STRUCTURAL (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P233" t="inlineStr">
@@ -21789,7 +21789,7 @@
       </c>
       <c r="O234" t="inlineStr">
         <is>
-          <t>STRUCTURAL (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P234" t="inlineStr">
@@ -21880,7 +21880,7 @@
       </c>
       <c r="O235" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P235" t="inlineStr">
@@ -21975,7 +21975,7 @@
       </c>
       <c r="O236" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (18)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P236" t="inlineStr">
@@ -22066,7 +22066,7 @@
       </c>
       <c r="O237" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (20), GLYCOPROTEIN (20), NUCLEOPROTEIN (20)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P237" t="inlineStr">
@@ -22157,7 +22157,7 @@
       </c>
       <c r="O238" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (18)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P238" t="inlineStr">
@@ -22248,7 +22248,7 @@
       </c>
       <c r="O239" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P239" t="inlineStr">
@@ -22343,7 +22343,7 @@
       </c>
       <c r="O240" t="inlineStr">
         <is>
-          <t>ENVELOPE (7)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P240" t="inlineStr">
@@ -22434,7 +22434,7 @@
       </c>
       <c r="O241" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (8)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P241" t="inlineStr">
@@ -22529,7 +22529,7 @@
       </c>
       <c r="O242" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P242" t="inlineStr">
@@ -22620,7 +22620,7 @@
       </c>
       <c r="O243" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P243" t="inlineStr">
@@ -22715,7 +22715,7 @@
       </c>
       <c r="O244" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (8)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P244" t="inlineStr">
@@ -22806,7 +22806,7 @@
       </c>
       <c r="O245" t="inlineStr">
         <is>
-          <t>L (1), GP (1), N (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P245" t="inlineStr">
@@ -22897,7 +22897,7 @@
       </c>
       <c r="O246" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1), GLYCOPROTEIN (1), RNA-DEPENDENT (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P246" t="inlineStr">
@@ -22984,7 +22984,7 @@
       </c>
       <c r="O247" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (8), NUCLEOPROTEIN (7)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P247" t="inlineStr">
@@ -23075,7 +23075,7 @@
       </c>
       <c r="O248" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P248" t="inlineStr">
@@ -23170,7 +23170,7 @@
       </c>
       <c r="O249" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1), ENVELOPE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P249" t="inlineStr">
@@ -23265,7 +23265,7 @@
       </c>
       <c r="O250" t="inlineStr">
         <is>
-          <t>L (1), GPC (1), N (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P250" t="inlineStr">
@@ -23356,7 +23356,7 @@
       </c>
       <c r="O251" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (8)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P251" t="inlineStr">
@@ -23451,7 +23451,7 @@
       </c>
       <c r="O252" t="inlineStr">
         <is>
-          <t>S (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P252" t="inlineStr">
@@ -23542,7 +23542,7 @@
       </c>
       <c r="O253" t="inlineStr">
         <is>
-          <t>S (27)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P253" t="inlineStr">
@@ -23633,7 +23633,7 @@
       </c>
       <c r="O254" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P254" t="inlineStr">
@@ -23720,7 +23720,7 @@
       </c>
       <c r="O255" t="inlineStr">
         <is>
-          <t>ENVELOPE (14)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P255" t="inlineStr">
@@ -23811,7 +23811,7 @@
       </c>
       <c r="O256" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (15)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P256" t="inlineStr">
@@ -23906,7 +23906,7 @@
       </c>
       <c r="O257" t="inlineStr">
         <is>
-          <t>L (1), ENVELOPE (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P257" t="inlineStr">
@@ -24001,7 +24001,7 @@
       </c>
       <c r="O258" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (16)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P258" t="inlineStr">
@@ -24092,7 +24092,7 @@
       </c>
       <c r="O259" t="inlineStr">
         <is>
-          <t>NP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P259" t="inlineStr">
@@ -24183,7 +24183,7 @@
       </c>
       <c r="O260" t="inlineStr">
         <is>
-          <t>N (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P260" t="inlineStr">
@@ -24278,7 +24278,7 @@
       </c>
       <c r="O261" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P261" t="inlineStr">
@@ -24373,7 +24373,7 @@
       </c>
       <c r="O262" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (6)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P262" t="inlineStr">
@@ -24468,7 +24468,7 @@
       </c>
       <c r="O263" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (8)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P263" t="inlineStr">
@@ -24559,7 +24559,7 @@
       </c>
       <c r="O264" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P264" t="inlineStr">
@@ -24654,7 +24654,7 @@
       </c>
       <c r="O265" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (6), ENVELOPE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P265" t="inlineStr">
@@ -24749,7 +24749,7 @@
       </c>
       <c r="O266" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P266" t="inlineStr">
@@ -24844,7 +24844,7 @@
       </c>
       <c r="O267" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P267" t="inlineStr">
@@ -24939,7 +24939,7 @@
       </c>
       <c r="O268" t="inlineStr">
         <is>
-          <t>ENVELOPE (1), NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P268" t="inlineStr">
@@ -25034,7 +25034,7 @@
       </c>
       <c r="O269" t="inlineStr">
         <is>
-          <t>N (13)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P269" t="inlineStr">
@@ -25129,7 +25129,7 @@
       </c>
       <c r="O270" t="inlineStr">
         <is>
-          <t>L (1), GLYCOPROTEIN (1), NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P270" t="inlineStr">
@@ -25224,7 +25224,7 @@
       </c>
       <c r="O271" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P271" t="inlineStr">
@@ -25315,7 +25315,7 @@
       </c>
       <c r="O272" t="inlineStr">
         <is>
-          <t>NP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P272" t="inlineStr">
@@ -25410,7 +25410,7 @@
       </c>
       <c r="O273" t="inlineStr">
         <is>
-          <t>POLYMERASE (1), GLYCOPROTEIN (1), NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P273" t="inlineStr">
@@ -25505,7 +25505,7 @@
       </c>
       <c r="O274" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (7), POLYMERASE (1), GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P274" t="inlineStr">
@@ -25596,7 +25596,7 @@
       </c>
       <c r="O275" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (24), GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P275" t="inlineStr">
@@ -25683,7 +25683,7 @@
       </c>
       <c r="O276" t="inlineStr">
         <is>
-          <t>ENVELOPE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P276" t="inlineStr">
@@ -25770,7 +25770,7 @@
       </c>
       <c r="O277" t="inlineStr">
         <is>
-          <t>ENVELOPE (6)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P277" t="inlineStr">
@@ -25861,7 +25861,7 @@
       </c>
       <c r="O278" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P278" t="inlineStr">
@@ -25952,7 +25952,7 @@
       </c>
       <c r="O279" t="inlineStr">
         <is>
-          <t>N (9)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P279" t="inlineStr">
@@ -26043,7 +26043,7 @@
       </c>
       <c r="O280" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (9)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P280" t="inlineStr">
@@ -26134,7 +26134,7 @@
       </c>
       <c r="O281" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (23), ENVELOPE (23), RNA-DEPENDENT (23)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P281" t="inlineStr">
@@ -26225,7 +26225,7 @@
       </c>
       <c r="O282" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P282" t="inlineStr">
@@ -26316,7 +26316,7 @@
       </c>
       <c r="O283" t="inlineStr">
         <is>
-          <t>S (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P283" t="inlineStr">
@@ -26407,7 +26407,7 @@
       </c>
       <c r="O284" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (1), POLYMERASE (1), NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P284" t="inlineStr">
@@ -26502,7 +26502,7 @@
       </c>
       <c r="O285" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (36), RNA-DEPENDENT (35), ENVELOPE (33)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P285" t="inlineStr">
@@ -26597,7 +26597,7 @@
       </c>
       <c r="O286" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (11)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P286" t="inlineStr">
@@ -26692,7 +26692,7 @@
       </c>
       <c r="O287" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P287" t="inlineStr">
@@ -26787,7 +26787,7 @@
       </c>
       <c r="O288" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (55), NUCLEOPROTEIN (55), POLYPROTEIN (31), RNA-DEPENDENT (12), PUTATIVE (10), L (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P288" t="inlineStr">
@@ -26878,7 +26878,7 @@
       </c>
       <c r="O289" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P289" t="inlineStr">
@@ -26973,7 +26973,7 @@
       </c>
       <c r="O290" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (15), S (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P290" t="inlineStr">
@@ -27064,7 +27064,7 @@
       </c>
       <c r="O291" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P291" t="inlineStr">
@@ -27155,7 +27155,7 @@
       </c>
       <c r="O292" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P292" t="inlineStr">
@@ -27246,7 +27246,7 @@
       </c>
       <c r="O293" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P293" t="inlineStr">
@@ -27337,7 +27337,7 @@
       </c>
       <c r="O294" t="inlineStr">
         <is>
-          <t>N (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P294" t="inlineStr">
@@ -27432,7 +27432,7 @@
       </c>
       <c r="O295" t="inlineStr">
         <is>
-          <t>ENVELOPE (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P295" t="inlineStr">
@@ -27523,7 +27523,7 @@
       </c>
       <c r="O296" t="inlineStr">
         <is>
-          <t>N (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P296" t="inlineStr">
@@ -27618,7 +27618,7 @@
       </c>
       <c r="O297" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (21)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P297" t="inlineStr">
@@ -27709,7 +27709,7 @@
       </c>
       <c r="O298" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P298" t="inlineStr">
@@ -27800,7 +27800,7 @@
       </c>
       <c r="O299" t="inlineStr">
         <is>
-          <t>N (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P299" t="inlineStr">
@@ -27895,7 +27895,7 @@
       </c>
       <c r="O300" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P300" t="inlineStr">
@@ -27986,7 +27986,7 @@
       </c>
       <c r="O301" t="inlineStr">
         <is>
-          <t>N (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P301" t="inlineStr">
@@ -28073,7 +28073,7 @@
       </c>
       <c r="O302" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P302" t="inlineStr">
@@ -28164,7 +28164,7 @@
       </c>
       <c r="O303" t="inlineStr">
         <is>
-          <t>NA (5)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P303" t="inlineStr">
@@ -28255,7 +28255,7 @@
       </c>
       <c r="O304" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (3), S (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P304" t="inlineStr">
@@ -28346,7 +28346,7 @@
       </c>
       <c r="O305" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1), S (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P305" t="inlineStr">
@@ -28437,7 +28437,7 @@
       </c>
       <c r="O306" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P306" t="inlineStr">
@@ -28528,7 +28528,7 @@
       </c>
       <c r="O307" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P307" t="inlineStr">
@@ -28619,7 +28619,7 @@
       </c>
       <c r="O308" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (25), NUCLEOPROTEIN (25)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P308" t="inlineStr">
@@ -28714,7 +28714,7 @@
       </c>
       <c r="O309" t="inlineStr">
         <is>
-          <t>S (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P309" t="inlineStr">
@@ -28809,7 +28809,7 @@
       </c>
       <c r="O310" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (55)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P310" t="inlineStr">
@@ -28896,7 +28896,7 @@
       </c>
       <c r="O311" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (11), RNA-DEPENDENT (11), NUCLEOCAPSID (11)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P311" t="inlineStr">
@@ -28987,7 +28987,7 @@
       </c>
       <c r="O312" t="inlineStr">
         <is>
-          <t>ENVELOPE (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P312" t="inlineStr">
@@ -29078,7 +29078,7 @@
       </c>
       <c r="O313" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2), GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P313" t="inlineStr">
@@ -29169,7 +29169,7 @@
       </c>
       <c r="O314" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1), NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P314" t="inlineStr">
@@ -29260,7 +29260,7 @@
       </c>
       <c r="O315" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (3)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P315" t="inlineStr">
@@ -29351,7 +29351,7 @@
       </c>
       <c r="O316" t="inlineStr">
         <is>
-          <t>NA (23), NUCLEOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P316" t="inlineStr">
@@ -29446,7 +29446,7 @@
       </c>
       <c r="O317" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (12), GLYCOPROTEIN (4), L (4)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P317" t="inlineStr">
@@ -29537,7 +29537,7 @@
       </c>
       <c r="O318" t="inlineStr">
         <is>
-          <t>S (7), M (7), RDRP (7)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P318" t="inlineStr">
@@ -29628,7 +29628,7 @@
       </c>
       <c r="O319" t="inlineStr">
         <is>
-          <t>ENVELOPE (14)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P319" t="inlineStr">
@@ -29719,7 +29719,7 @@
       </c>
       <c r="O320" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN, NUCLEOPROTEIN (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P320" t="inlineStr">
@@ -29814,7 +29814,7 @@
       </c>
       <c r="O321" t="inlineStr">
         <is>
-          <t>NUCLEOPROTEIN (1), GLYCOPROTEIN (1), RNA-DEPENDENT (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P321" t="inlineStr">
@@ -29905,7 +29905,7 @@
       </c>
       <c r="O322" t="inlineStr">
         <is>
-          <t>STRUCTURAL (11)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P322" t="inlineStr">
@@ -29992,7 +29992,7 @@
       </c>
       <c r="O323" t="inlineStr">
         <is>
-          <t>RNA-DEPENDENT (1), GLYCOPROTEIN (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P323" t="inlineStr">
@@ -30083,7 +30083,7 @@
       </c>
       <c r="O324" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (1), PREGLYCOPROTEIN (1), L (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P324" t="inlineStr">
@@ -30178,7 +30178,7 @@
       </c>
       <c r="O325" t="inlineStr">
         <is>
-          <t>NUCLEOCAPSID (2), GLYCOPROTEIN (2), RNA-DEPENDENT (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P325" t="inlineStr">
@@ -30269,7 +30269,7 @@
       </c>
       <c r="O326" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (2), NUCLEOCAPSID (2), RNA-DEPENDENT (2)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P326" t="inlineStr">
@@ -30360,7 +30360,7 @@
       </c>
       <c r="O327" t="inlineStr">
         <is>
-          <t>GLYCOPROTEIN (16), NUCLEOPROTEIN (16), L (16)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P327" t="inlineStr">
@@ -30455,7 +30455,7 @@
       </c>
       <c r="O328" t="inlineStr">
         <is>
-          <t>NA (2), NP (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P328" t="inlineStr">
@@ -30550,7 +30550,7 @@
       </c>
       <c r="O329" t="inlineStr">
         <is>
-          <t>NP (5), RDRP (1), GPC (1)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P329" t="inlineStr">

</xml_diff>